<commit_message>
Merged PR 15345: BP-4428-Result reports need to indicate that fluidity is being utilized
Result reports need to indicate that fluidity is being utilized
</commit_message>
<xml_diff>
--- a/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Pricing Results.xlsx
+++ b/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Pricing Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\achyzh\Broadcast\Source\Tam\Maestro\UI\BroadcastComposerWeb\App_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\Source\Tam\Maestro\UI\BroadcastComposerWeb\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0515B0D-E462-42A7-8D38-115AD347249D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C557A95D-EBA8-47BA-A6BD-215662FBC6CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="705" yWindow="600" windowWidth="27360" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="9720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Allocations" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Total Cost</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>Total Impressions</t>
+  </si>
+  <si>
+    <t>Fluidity</t>
   </si>
 </sst>
 </file>
@@ -487,7 +490,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -549,6 +552,9 @@
       </c>
       <c r="F4" s="17" t="s">
         <v>2</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -17252,7 +17258,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;A</oddHeader>
     <oddFooter>Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Merged PR 16386: BP-4928-Result Export - Add "Affiliate" column for every row and populate (Buying and Planning)
Result Export - Add "Affiliate" column for every row and populate (Buying and Planning)
</commit_message>
<xml_diff>
--- a/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Pricing Results.xlsx
+++ b/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Pricing Results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\Source\Tam\Maestro\UI\BroadcastComposerWeb\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C557A95D-EBA8-47BA-A6BD-215662FBC6CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E2D4115-4297-45CA-A503-16A73F74D198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="9720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Total Cost</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>Fluidity</t>
+  </si>
+  <si>
+    <t>Affiliate</t>
   </si>
 </sst>
 </file>
@@ -486,11 +489,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O986"/>
+  <dimension ref="A1:P986"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -512,7 +515,7 @@
     <col min="15" max="15" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
         <v>4</v>
       </c>
@@ -522,7 +525,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>5</v>
       </c>
@@ -532,14 +535,14 @@
       <c r="E2" s="6"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
       <c r="C4" s="16" t="s">
         <v>1</v>
@@ -557,7 +560,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
         <v>3</v>
       </c>
@@ -566,7 +569,7 @@
       <c r="E5" s="25"/>
       <c r="F5" s="25"/>
     </row>
-    <row r="7" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
         <v>10</v>
       </c>
@@ -580,40 +583,43 @@
         <v>15</v>
       </c>
       <c r="E7" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="G7" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="18" t="s">
+      <c r="H7" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="19" t="s">
+      <c r="I7" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="I7" s="20" t="s">
+      <c r="J7" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="J7" s="20" t="s">
+      <c r="K7" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="K7" s="21" t="s">
+      <c r="L7" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="L7" s="22" t="s">
+      <c r="M7" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="M7" s="18" t="s">
+      <c r="N7" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="N7" s="22" t="s">
+      <c r="O7" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="O7" s="18" t="s">
+      <c r="P7" s="18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -630,7 +636,7 @@
       <c r="N8" s="13"/>
       <c r="O8" s="1"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -647,7 +653,7 @@
       <c r="N9" s="13"/>
       <c r="O9" s="9"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -664,7 +670,7 @@
       <c r="N10" s="13"/>
       <c r="O10" s="9"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -681,7 +687,7 @@
       <c r="N11" s="13"/>
       <c r="O11" s="9"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -698,7 +704,7 @@
       <c r="N12" s="13"/>
       <c r="O12" s="9"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -715,7 +721,7 @@
       <c r="N13" s="13"/>
       <c r="O13" s="9"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -732,7 +738,7 @@
       <c r="N14" s="13"/>
       <c r="O14" s="9"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -749,7 +755,7 @@
       <c r="N15" s="13"/>
       <c r="O15" s="9"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>

</xml_diff>